<commit_message>
"Get visiting chart data from gymAdmin" logic in progress. Part 4
Read data from Excel and save to DB complete.
</commit_message>
<xml_diff>
--- a/FitMeApp/wwwroot/ExcelFiles/Chars/BigRock/VisitingChart.xlsx
+++ b/FitMeApp/wwwroot/ExcelFiles/Chars/BigRock/VisitingChart.xlsx
@@ -47,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -67,8 +67,13 @@
       <scheme val="minor"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF161616"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +96,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF93C47D"/>
         <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -152,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -187,6 +198,9 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -743,49 +757,49 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="14">
         <v>0.0</v>
       </c>
       <c r="C9" s="12">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="14">
         <v>0.0</v>
       </c>
       <c r="E9" s="12">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="14">
         <v>0.0</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="14">
         <v>0.0</v>
       </c>
       <c r="I9" s="12">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="14">
         <v>0.0</v>
       </c>
       <c r="K9" s="13">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="14">
         <v>0.0</v>
       </c>
       <c r="M9" s="13">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="N9" s="10">
+      <c r="N9" s="14">
         <v>0.0</v>
       </c>
     </row>
@@ -897,42 +911,42 @@
         <v>8</v>
       </c>
       <c r="B12" s="10">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="D12" s="10">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="E12" s="12">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="F12" s="10">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="G12" s="12">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="H12" s="10">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="I12" s="12">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="J12" s="10">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="K12" s="13">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="L12" s="10">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="M12" s="13">
         <f t="shared" si="7"/>
@@ -948,49 +962,49 @@
         <v>9</v>
       </c>
       <c r="B13" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="C13" s="12">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="D13" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="E13" s="12">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="F13" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="G13" s="12">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="H13" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="I13" s="12">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="J13" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="K13" s="13">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="L13" s="10">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="M13" s="13">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="N13" s="10">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="14">
@@ -999,49 +1013,49 @@
         <v>10</v>
       </c>
       <c r="B14" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="C14" s="12">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="D14" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="E14" s="12">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="F14" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="G14" s="12">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="H14" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="I14" s="12">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J14" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="K14" s="13">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="L14" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="M14" s="13">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="N14" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="15">
@@ -1050,49 +1064,49 @@
         <v>11</v>
       </c>
       <c r="B15" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="D15" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="E15" s="12">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="F15" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="G15" s="12">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="H15" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="I15" s="12">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="J15" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="K15" s="13">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="L15" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="M15" s="13">
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="N15" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="16">
@@ -1101,49 +1115,49 @@
         <v>12</v>
       </c>
       <c r="B16" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="D16" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="E16" s="12">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="F16" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="G16" s="12">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="H16" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="I16" s="12">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="J16" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="K16" s="13">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="L16" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="M16" s="13">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="N16" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="17">
@@ -1152,49 +1166,49 @@
         <v>13</v>
       </c>
       <c r="B17" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="C17" s="12">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="D17" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="E17" s="12">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="F17" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="G17" s="12">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="H17" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="I17" s="12">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="J17" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="K17" s="13">
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="L17" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="M17" s="13">
         <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="N17" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="18">
@@ -1203,49 +1217,49 @@
         <v>14</v>
       </c>
       <c r="B18" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="C18" s="12">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="D18" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="E18" s="12">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="F18" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="G18" s="12">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="H18" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="I18" s="12">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="J18" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="K18" s="13">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="L18" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="M18" s="13">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="N18" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="19">
@@ -1254,49 +1268,49 @@
         <v>15</v>
       </c>
       <c r="B19" s="10">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="D19" s="10">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="E19" s="12">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="F19" s="10">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="G19" s="12">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="H19" s="10">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="I19" s="12">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="J19" s="10">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="K19" s="13">
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="L19" s="10">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="M19" s="13">
         <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="N19" s="10">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="20">
@@ -1305,49 +1319,49 @@
         <v>16</v>
       </c>
       <c r="B20" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="C20" s="12">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="D20" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="E20" s="12">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="F20" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="G20" s="12">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="H20" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="I20" s="12">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J20" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="K20" s="13">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="L20" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="M20" s="13">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="N20" s="10">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="21">
@@ -1356,49 +1370,49 @@
         <v>17</v>
       </c>
       <c r="B21" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="C21" s="12">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="D21" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="E21" s="12">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="F21" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="G21" s="12">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="H21" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="I21" s="12">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="J21" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="K21" s="13">
         <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="L21" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="M21" s="13">
         <f t="shared" si="7"/>
         <v>17</v>
       </c>
       <c r="N21" s="10">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="22">
@@ -1407,49 +1421,49 @@
         <v>18</v>
       </c>
       <c r="B22" s="10">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="C22" s="12">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="D22" s="10">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="E22" s="12">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="F22" s="10">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="G22" s="12">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="H22" s="10">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="J22" s="10">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="K22" s="13">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="L22" s="10">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="M22" s="13">
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="N22" s="10">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="23">
@@ -1458,49 +1472,49 @@
         <v>19</v>
       </c>
       <c r="B23" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="C23" s="12">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="D23" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="E23" s="12">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="F23" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="G23" s="12">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="H23" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="I23" s="12">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="J23" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="K23" s="13">
         <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="L23" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="M23" s="13">
         <f t="shared" si="7"/>
         <v>19</v>
       </c>
       <c r="N23" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="24">
@@ -1509,49 +1523,49 @@
         <v>20</v>
       </c>
       <c r="B24" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="C24" s="12">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="D24" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="E24" s="12">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="F24" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="G24" s="12">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="H24" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="I24" s="12">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="J24" s="10">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="K24" s="13">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="L24" s="10">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="M24" s="13">
         <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="N24" s="10">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="25">
@@ -1560,35 +1574,35 @@
         <v>21</v>
       </c>
       <c r="B25" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="C25" s="12">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="D25" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="E25" s="12">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="F25" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="G25" s="12">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="H25" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="I25" s="12">
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="J25" s="10">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="K25" s="13">
         <f t="shared" si="6"/>
@@ -1611,35 +1625,35 @@
         <v>22</v>
       </c>
       <c r="B26" s="10">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="C26" s="12">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="D26" s="10">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="E26" s="12">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="F26" s="10">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="G26" s="12">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="H26" s="10">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="I26" s="12">
         <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="J26" s="10">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="K26" s="13">
         <f t="shared" si="6"/>
@@ -1657,53 +1671,53 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="14">
+      <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B27" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="C27" s="14">
+      <c r="B27" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="C27" s="15">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="D27" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="E27" s="14">
+      <c r="D27" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="E27" s="15">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="F27" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="G27" s="14">
+      <c r="F27" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="G27" s="15">
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="H27" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="I27" s="14">
+      <c r="H27" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="I27" s="15">
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
-      <c r="J27" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="K27" s="16">
+      <c r="J27" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="K27" s="17">
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="L27" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="M27" s="16">
+      <c r="L27" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="M27" s="17">
         <f t="shared" si="7"/>
         <v>23</v>
       </c>
-      <c r="N27" s="15">
+      <c r="N27" s="16">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>